<commit_message>
Added playlist functionality, can create/del lists and add/remove movies
</commit_message>
<xml_diff>
--- a/Self-Assessment-Rubric.xlsx
+++ b/Self-Assessment-Rubric.xlsx
@@ -1337,7 +1337,36 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>A playlist page has been added (see playlistPage.js) plus related functionality i.e. add to playlist button appears on movie cards; delete button shows on the playlist page so that movies can be removed from the playlist. </a:t>
+            <a:t>A playlist page has been added (see playlistPage.jsx) plus related functionality i.e. playlist button on cards opens dialog with multiple options. Can create or delete playlists. Can add or remove movies from playlists</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Can search for movies or actors. Can filter alphabetically, age, release date, ratings…….</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1681,7 +1710,7 @@
   </sheetPr>
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added recommendations to movieDetails. Added style changes to filter card layout and image. Updated app theme/colours
</commit_message>
<xml_diff>
--- a/Self-Assessment-Rubric.xlsx
+++ b/Self-Assessment-Rubric.xlsx
@@ -219,17 +219,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0%"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0%"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -350,6 +352,12 @@
       <name val="Calibri"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -361,43 +369,43 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor rgb="FFC6BAD6"/>
+        <bgColor rgb="FFC9211E"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor rgb="FF800080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFA33E03"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor rgb="FFF79646"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor rgb="FF99CC00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.5999"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.5999"/>
-        <bgColor rgb="FFBDD7EE"/>
+        <bgColor rgb="FFE3AEAD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.5999"/>
-        <bgColor rgb="FFC5E0B4"/>
+        <bgColor rgb="FFFABF8F"/>
       </patternFill>
     </fill>
     <fill>
@@ -409,7 +417,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC0504D"/>
-        <bgColor rgb="FF993366"/>
+        <bgColor rgb="FFA33E03"/>
       </patternFill>
     </fill>
     <fill>
@@ -421,7 +429,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
-        <bgColor rgb="FF0563C1"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
@@ -433,7 +441,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE3AEAD"/>
-        <bgColor rgb="FFFABF8F"/>
+        <bgColor rgb="FFF19F9E"/>
       </patternFill>
     </fill>
     <fill>
@@ -517,30 +525,52 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -552,43 +582,43 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -596,23 +626,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -628,11 +658,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="9" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="9" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -640,11 +670,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -660,7 +690,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="16" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="16" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -668,23 +698,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -711,7 +741,7 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
@@ -719,18 +749,18 @@
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF0070C0"/>
+      <rgbColor rgb="FF8E03A3"/>
+      <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC6BAD6"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF5B9BD5"/>
+      <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FFC0504D"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0563C1"/>
-      <rgbColor rgb="FFBDD7EE"/>
+      <rgbColor rgb="FF0070C0"/>
+      <rgbColor rgb="FFE3AEAD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -741,26 +771,26 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFC5E0B4"/>
-      <rgbColor rgb="FFFFE699"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFE383"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFE3AEAD"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFF19F9E"/>
+      <rgbColor rgb="FFEB78FD"/>
       <rgbColor rgb="FFFABF8F"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFC000"/>
+      <rgbColor rgb="FFC99C00"/>
+      <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFF79646"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF8064A2"/>
-      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF70AD47"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFA33E03"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF595959"/>
     </indexedColors>
@@ -779,9 +809,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1294920</xdr:colOff>
+      <xdr:colOff>1294560</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>342000</xdr:rowOff>
+      <xdr:rowOff>341640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -791,7 +821,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6667200" y="1524600"/>
-          <a:ext cx="4242240" cy="694440"/>
+          <a:ext cx="4241880" cy="694080"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
           <a:avLst>
@@ -804,10 +834,7 @@
         </a:solidFill>
         <a:ln w="12700">
           <a:solidFill>
-            <a:srgbClr val="000000">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:srgbClr>
+            <a:srgbClr val="595959"/>
           </a:solidFill>
           <a:miter/>
         </a:ln>
@@ -842,6 +869,7 @@
                 <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>Add links to your GitHub repo and demo video</a:t>
           </a:r>
@@ -862,9 +890,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1313280</xdr:colOff>
+      <xdr:colOff>1312920</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>38880</xdr:rowOff>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -874,7 +902,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7657920" y="552960"/>
-          <a:ext cx="3269880" cy="791640"/>
+          <a:ext cx="3269520" cy="791280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -884,10 +912,7 @@
         </a:solidFill>
         <a:ln w="12700">
           <a:solidFill>
-            <a:srgbClr val="000000">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:srgbClr>
+            <a:srgbClr val="595959"/>
           </a:solidFill>
           <a:miter/>
         </a:ln>
@@ -922,6 +947,7 @@
                 <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>After filling in this sheet, save it with the filename YOURNAME_CA1.xslx and upload it to Moodle</a:t>
           </a:r>
@@ -942,9 +968,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>5038200</xdr:colOff>
+      <xdr:colOff>5037840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:rowOff>6840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -954,7 +980,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11959560" y="3743280"/>
-          <a:ext cx="7876800" cy="1907640"/>
+          <a:ext cx="7876800" cy="1907280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -964,9 +990,7 @@
         </a:solidFill>
         <a:ln w="9525">
           <a:solidFill>
-            <a:srgbClr val="ffffff">
-              <a:shade val="50000"/>
-            </a:srgbClr>
+            <a:srgbClr val="bcbcbc"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -993,6 +1017,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>Added the following static routes:</a:t>
           </a:r>
@@ -1012,6 +1037,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>  </a:t>
           </a:r>
@@ -1021,6 +1047,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>/top-rated (topRatedMoviesPage.js)</a:t>
           </a:r>
@@ -1040,6 +1067,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>  </a:t>
           </a:r>
@@ -1049,6 +1077,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>/trending (trendingMovies.js)</a:t>
           </a:r>
@@ -1068,6 +1097,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>  </a:t>
           </a:r>
@@ -1077,6 +1107,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>/upcoming (upcomingMovies.js)</a:t>
           </a:r>
@@ -1096,6 +1127,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>Also added parameterised routes (movies and actors are internally linked):</a:t>
           </a:r>
@@ -1115,6 +1147,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>  </a:t>
           </a:r>
@@ -1124,6 +1157,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>/movie/:id/videos (shows up to 3 official english trailers – movieDetailsPage.jsx)</a:t>
           </a:r>
@@ -1143,6 +1177,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>  </a:t>
           </a:r>
@@ -1152,6 +1187,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>/movie/:id/credits (the list of cast for a movie - movieDetailsPage.jsx)</a:t>
           </a:r>
@@ -1171,6 +1207,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>  </a:t>
           </a:r>
@@ -1180,6 +1217,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>/movie/:id/recommendations (list of recommended movies – movieDetailsPage.jsx</a:t>
           </a:r>
@@ -1199,6 +1237,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>  </a:t>
           </a:r>
@@ -1208,6 +1247,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>/person:id (display actor details – personDetailsPage.jsx)</a:t>
           </a:r>
@@ -1227,6 +1267,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>  </a:t>
           </a:r>
@@ -1236,6 +1277,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>/person:id/moviecredits (display movies actor has starred in – personDetailsPage.jsx)</a:t>
           </a:r>
@@ -1256,9 +1298,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>5038200</xdr:colOff>
+      <xdr:colOff>5037840</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1268,7 +1310,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11959560" y="6196680"/>
-          <a:ext cx="7876800" cy="1907640"/>
+          <a:ext cx="7876800" cy="1907280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1278,9 +1320,7 @@
         </a:solidFill>
         <a:ln w="9525">
           <a:solidFill>
-            <a:srgbClr val="ffffff">
-              <a:shade val="50000"/>
-            </a:srgbClr>
+            <a:srgbClr val="bcbcbc"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -1307,6 +1347,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>All new endpoints use react-query caching</a:t>
           </a:r>
@@ -1336,8 +1377,9 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>A playlist page has been added (see playlistPage.jsx) plus related functionality i.e. playlist button on cards opens dialog with multiple options. Can create or delete playlists. Can add or remove movies from playlists</a:t>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:rPr>
+            <a:t>A playlist page has been added (see playlistPage.jsx) with functionality i.e. playlist button on cards opens dialog with multiple options. Can create or delete playlists. Can add or remove movies from playlists</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1365,8 +1407,9 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Can search for movies or actors. Can filter alphabetically, age, release date, ratings…….</a:t>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:rPr>
+            <a:t>Can search for movies or actors. Can filter movies alphabetically, release date rating or popularity. Can filter people alphabetically, age or total movie count</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1385,9 +1428,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>5033520</xdr:colOff>
+      <xdr:colOff>5033160</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1902960</xdr:rowOff>
+      <xdr:rowOff>1902600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1397,7 +1440,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11954880" y="8636040"/>
-          <a:ext cx="7876800" cy="1902960"/>
+          <a:ext cx="7876800" cy="1902600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1407,9 +1450,7 @@
         </a:solidFill>
         <a:ln w="9525">
           <a:solidFill>
-            <a:srgbClr val="ffffff">
-              <a:shade val="50000"/>
-            </a:srgbClr>
+            <a:srgbClr val="bcbcbc"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -1436,6 +1477,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>Changed the app's colour scheme.</a:t>
           </a:r>
@@ -1455,6 +1497,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>Replaced the image on filter card.</a:t>
           </a:r>
@@ -1474,8 +1517,9 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Added pagination on all movie list pages.</a:t>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:rPr>
+            <a:t>Added pagination on all movie list pages and playlist page</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1493,6 +1537,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>Used MUI pagination component to display numbers. </a:t>
           </a:r>
@@ -1513,9 +1558,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>5033520</xdr:colOff>
+      <xdr:colOff>5033160</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>1902960</xdr:rowOff>
+      <xdr:rowOff>1902600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1525,7 +1570,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11954880" y="11084760"/>
-          <a:ext cx="7876800" cy="1902600"/>
+          <a:ext cx="7876800" cy="1902240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1535,9 +1580,7 @@
         </a:solidFill>
         <a:ln w="9525">
           <a:solidFill>
-            <a:srgbClr val="ffffff">
-              <a:shade val="50000"/>
-            </a:srgbClr>
+            <a:srgbClr val="bcbcbc"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -1564,6 +1607,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>Video has been recorded and includes a voiceover. </a:t>
           </a:r>
@@ -1583,6 +1627,7 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
             <a:t>This document has been completed with all required details (with brief descriptions). </a:t>
           </a:r>
@@ -1710,7 +1755,7 @@
   </sheetPr>
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -1721,86 +1766,86 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="18.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="2" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="12.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="40.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="40.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="80.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="1" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="34.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="1" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="19" style="2" width="12.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="14.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="K1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="K3" s="7" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="K3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="T3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="U3" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6" t="n">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="n">
         <v>20012345</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="K4" s="11" t="str">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="K4" s="12" t="str">
         <f aca="false">IF(U10&gt;0, _xlfn.CONCAT(ROUND(S10, 0), " - ", ROUND(T10, 0), "%"), "")</f>
         <v>85 - 100%</v>
       </c>
@@ -1808,7 +1853,7 @@
         <f aca="false">A15</f>
         <v>1. Extend the app</v>
       </c>
-      <c r="P4" s="12" t="n">
+      <c r="P4" s="13" t="n">
         <f aca="false">B15</f>
         <v>40</v>
       </c>
@@ -1816,31 +1861,31 @@
         <f aca="false">IF(H16,$H$12,IF(G16,$G$12,IF(F16,$F$12,IF(E16,$E$12,IF(D16,$D$12,IF(C16,$C$12, ""))))))</f>
         <v>Outstanding</v>
       </c>
-      <c r="R4" s="13" t="str">
+      <c r="R4" s="14" t="str">
         <f aca="false">IF(H16,$H$13,IF(G16,$G$13,IF(F16,$F$13,IF(E16,$E$13,IF(D16,$D$13,IF(C16,$C$13,""))))))</f>
         <v>85% - 100%</v>
       </c>
-      <c r="S4" s="12" t="n">
+      <c r="S4" s="13" t="n">
         <f aca="false">IF(Q4="Outstanding",P4*85%,IF(Q4="Excellent",P4*70%,IF(Q4="Good",P4*55%,IF(Q4="Baseline",P4*40%,IF(Q4="Below baseline",P4*20%,IF(Q4="Incomplete",P4*0%,""))))))</f>
         <v>34</v>
       </c>
-      <c r="T4" s="12" t="n">
+      <c r="T4" s="13" t="n">
         <f aca="false">IF(Q4="Outstanding",P4*100%,IF(Q4="Excellent",P4*84%,IF(Q4="Good",P4*69%,IF(Q4="Baseline",P4*54%,IF(Q4="Below baseline",P4*39%, IF(Q4="Incomplete",P4*19%,""))))))</f>
         <v>40</v>
       </c>
-      <c r="U4" s="12" t="n">
+      <c r="U4" s="13" t="n">
         <f aca="false">IF(COUNT(S4:T4)&gt;0, SUM(S4:T4)/2, "")</f>
         <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="O5" s="1" t="str">
         <f aca="false">A18</f>
         <v>2. Extend the functionality</v>
       </c>
-      <c r="P5" s="12" t="n">
+      <c r="P5" s="13" t="n">
         <f aca="false">B18</f>
         <v>25</v>
       </c>
@@ -1852,37 +1897,37 @@
         <f aca="false">IF(H19,$H$13,IF(G19,$G$13,IF(F19,$F$13,IF(E19,$E$13,IF(D19,$D$13,IF(C19,$C$13,""))))))</f>
         <v>85% - 100%</v>
       </c>
-      <c r="S5" s="12" t="n">
+      <c r="S5" s="13" t="n">
         <f aca="false">IF(Q5="Outstanding",P5*85%,IF(Q5="Excellent",P5*70%,IF(Q5="Good",P5*55%,IF(Q5="Baseline",P5*40%,IF(Q5="Below baseline",P5*20%,IF(Q5="Incomplete",P5*0%,""))))))</f>
         <v>21.25</v>
       </c>
-      <c r="T5" s="12" t="n">
+      <c r="T5" s="13" t="n">
         <f aca="false">IF(Q5="Outstanding",P5*100%,IF(Q5="Excellent",P5*84%,IF(Q5="Good",P5*69%,IF(Q5="Baseline",P5*54%,IF(Q5="Below baseline",P5*39%, IF(Q5="Incomplete",P5*19%,""))))))</f>
         <v>25</v>
       </c>
-      <c r="U5" s="12" t="n">
+      <c r="U5" s="13" t="n">
         <f aca="false">IF(COUNT(S5:T5)&gt;0, SUM(S5:T5)/2, "")</f>
         <v>23.125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="16" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="K6" s="17" t="s">
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="K6" s="18" t="s">
         <v>16</v>
       </c>
       <c r="O6" s="1" t="str">
         <f aca="false">A21</f>
         <v>3. Additional work</v>
       </c>
-      <c r="P6" s="12" t="n">
+      <c r="P6" s="13" t="n">
         <f aca="false">B21</f>
         <v>25</v>
       </c>
@@ -1894,34 +1939,34 @@
         <f aca="false">IF(H22,$H$13,IF(G22,$G$13,IF(F22,$F$13,IF(E22,$E$13,IF(D22,$D$13,IF(C22,$C$13,""))))))</f>
         <v>85% - 100%</v>
       </c>
-      <c r="S6" s="12" t="n">
+      <c r="S6" s="13" t="n">
         <f aca="false">IF(Q6="Outstanding",P6*85%,IF(Q6="Excellent",P6*70%,IF(Q6="Good",P6*55%,IF(Q6="Baseline",P6*40%,IF(Q6="Below baseline",P6*20%,IF(Q6="Incomplete",P6*0%,""))))))</f>
         <v>21.25</v>
       </c>
-      <c r="T6" s="12" t="n">
+      <c r="T6" s="13" t="n">
         <f aca="false">IF(Q6="Outstanding",P6*100%,IF(Q6="Excellent",P6*84%,IF(Q6="Good",P6*69%,IF(Q6="Baseline",P6*54%,IF(Q6="Below baseline",P6*39%, IF(Q6="Incomplete",P6*19%,""))))))</f>
         <v>25</v>
       </c>
-      <c r="U6" s="12" t="n">
+      <c r="U6" s="13" t="n">
         <f aca="false">IF(COUNT(S6:T6)&gt;0, SUM(S6:T6)/2, "")</f>
         <v>23.125</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
       <c r="O7" s="1" t="str">
         <f aca="false">A24</f>
         <v>4. Documentation and demo video</v>
       </c>
-      <c r="P7" s="12" t="n">
+      <c r="P7" s="13" t="n">
         <f aca="false">B24</f>
         <v>10</v>
       </c>
@@ -1933,83 +1978,83 @@
         <f aca="false">IF(H25,$H$13,IF(G25,$G$13,IF(F25,$F$13,IF(E25,$E$13,IF(D25,$D$13,IF(C25,$C$13,""))))))</f>
         <v>85% - 100%</v>
       </c>
-      <c r="S7" s="12" t="n">
+      <c r="S7" s="13" t="n">
         <f aca="false">IF(Q7="Outstanding",P7*85%,IF(Q7="Excellent",P7*70%,IF(Q7="Good",P7*55%,IF(Q7="Baseline",P7*40%,IF(Q7="Below baseline",P7*20%,IF(Q7="Incomplete",P7*0%,""))))))</f>
         <v>8.5</v>
       </c>
-      <c r="T7" s="12" t="n">
+      <c r="T7" s="13" t="n">
         <f aca="false">IF(Q7="Outstanding",P7*100%,IF(Q7="Excellent",P7*84%,IF(Q7="Good",P7*69%,IF(Q7="Baseline",P7*54%,IF(Q7="Below baseline",P7*39%, IF(Q7="Incomplete",P7*19%,""))))))</f>
         <v>10</v>
       </c>
-      <c r="U7" s="12" t="n">
+      <c r="U7" s="13" t="n">
         <f aca="false">IF(COUNT(S7:T7)&gt;0, SUM(S7:T7)/2, "")</f>
         <v>9.25</v>
       </c>
-      <c r="V7" s="18"/>
+      <c r="V7" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R9" s="19" t="s">
+      <c r="R9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="S9" s="10" t="s">
+      <c r="S9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="T9" s="10" t="s">
+      <c r="T9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="U9" s="10" t="s">
+      <c r="U9" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="J10" s="4" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="J10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="S10" s="12" t="n">
+      <c r="K10" s="5"/>
+      <c r="S10" s="13" t="n">
         <f aca="false">IF(COUNTBLANK($Q$4:$Q$7)&gt;3,0, SUM(S4:S7))</f>
         <v>85</v>
       </c>
-      <c r="T10" s="12" t="n">
+      <c r="T10" s="13" t="n">
         <f aca="false">IF(COUNTBLANK($Q$4:$Q$7)&gt;3, 0, SUM(T4:T7))</f>
         <v>100</v>
       </c>
-      <c r="U10" s="12" t="n">
+      <c r="U10" s="13" t="n">
         <f aca="false">IF(COUNTBLANK($Q$4:$Q$7)&gt;3, 0, SUM(U4:U7))</f>
         <v>92.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="20" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="26" t="s">
         <v>31</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -2017,27 +2062,27 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26" t="n">
+      <c r="A13" s="27" t="n">
         <f aca="false">SUM(B15:B25)</f>
         <v>100</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28" t="s">
+      <c r="B13" s="28"/>
+      <c r="C13" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="34" t="s">
         <v>38</v>
       </c>
       <c r="J13" s="2" t="s">
@@ -2045,265 +2090,265 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="35" t="n">
+      <c r="B15" s="36" t="n">
         <v>40</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="38" t="n">
+      <c r="B16" s="38"/>
+      <c r="C16" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D16" s="38" t="n">
+      <c r="D16" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E16" s="38" t="n">
+      <c r="E16" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F16" s="38" t="n">
+      <c r="F16" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G16" s="38" t="n">
+      <c r="G16" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H16" s="38" t="n">
+      <c r="H16" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J16" s="39" t="str">
+      <c r="J16" s="40" t="str">
         <f aca="false">IF(H16,$H$12,IF(G16,$G$12,IF(F16,$F$12,IF(E16,$E$12,IF(D16,$D$12,IF(C16,$C$12,"Please check one of the options"))))))</f>
         <v>Outstanding</v>
       </c>
-      <c r="K16" s="39" t="str">
+      <c r="K16" s="40" t="str">
         <f aca="false">IF(H16,$H$13,IF(G16,$G$13,IF(F16,$F$13,IF(E16,$E$13,IF(D16,$D$13,IF(C16,$C$13,""))))))</f>
         <v>85% - 100%</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="35" t="n">
+      <c r="B18" s="36" t="n">
         <v>25</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="38" t="n">
+      <c r="B19" s="38"/>
+      <c r="C19" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D19" s="38" t="n">
+      <c r="D19" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E19" s="38" t="n">
+      <c r="E19" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F19" s="38" t="n">
+      <c r="F19" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G19" s="38" t="n">
+      <c r="G19" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H19" s="38" t="n">
+      <c r="H19" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J19" s="39" t="str">
+      <c r="J19" s="40" t="str">
         <f aca="false">IF(H19,$H$12,IF(G19,$G$12,IF(F19,$F$12,IF(E19,$E$12,IF(D19,$D$12,IF(C19,$C$12,"Please check one of the options"))))))</f>
         <v>Outstanding</v>
       </c>
-      <c r="K19" s="39" t="str">
+      <c r="K19" s="40" t="str">
         <f aca="false">IF(H19,$H$13,IF(G19,$G$13,IF(F19,$F$13,IF(E19,$E$13,IF(D19,$D$13,IF(C19,$C$13,""))))))</f>
         <v>85% - 100%</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="35" t="n">
+      <c r="B21" s="36" t="n">
         <v>25</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
     </row>
     <row r="22" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="38" t="n">
+      <c r="B22" s="38"/>
+      <c r="C22" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D22" s="38" t="n">
+      <c r="D22" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E22" s="38" t="n">
+      <c r="E22" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F22" s="38" t="n">
+      <c r="F22" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G22" s="38" t="n">
+      <c r="G22" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H22" s="38" t="n">
+      <c r="H22" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J22" s="39" t="str">
+      <c r="J22" s="40" t="str">
         <f aca="false">IF(H22,$H$12,IF(G22,$G$12,IF(F22,$F$12,IF(E22,$E$12,IF(D22,$D$12,IF(C22,$C$12,"Please check one of the options"))))))</f>
         <v>Outstanding</v>
       </c>
-      <c r="K22" s="39" t="str">
+      <c r="K22" s="40" t="str">
         <f aca="false">IF(H22,$H$13,IF(G22,$G$13,IF(F22,$F$13,IF(E22,$E$13,IF(D22,$D$13,IF(C22,$C$13,""))))))</f>
         <v>85% - 100%</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="35" t="n">
+      <c r="B24" s="36" t="n">
         <v>10</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="32" t="s">
+      <c r="G24" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="H24" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="37"/>
-      <c r="C25" s="38" t="n">
+      <c r="B25" s="38"/>
+      <c r="C25" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D25" s="38" t="n">
+      <c r="D25" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E25" s="38" t="n">
+      <c r="E25" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F25" s="38" t="n">
+      <c r="F25" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G25" s="38" t="n">
+      <c r="G25" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H25" s="38" t="n">
+      <c r="H25" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J25" s="39" t="str">
+      <c r="J25" s="40" t="str">
         <f aca="false">IF(H25,$H$12,IF(G25,$G$12,IF(F25,$F$12,IF(E25,$E$12,IF(D25,$D$12,IF(C25,$C$12,"Please check one of the options"))))))</f>
         <v>Outstanding</v>
       </c>
-      <c r="K25" s="39" t="str">
+      <c r="K25" s="40" t="str">
         <f aca="false">IF(H25,$H$13,IF(G25,$G$13,IF(F25,$F$13,IF(E25,$E$13,IF(D25,$D$13,IF(C25,$C$13,""))))))</f>
         <v>85% - 100%</v>
       </c>

</xml_diff>

<commit_message>
Fixed navigation issues on pages
</commit_message>
<xml_diff>
--- a/Self-Assessment-Rubric.xlsx
+++ b/Self-Assessment-Rubric.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">A.N. Other</t>
+    <t xml:space="preserve">Ryan O’Loughlin</t>
   </si>
   <si>
     <t xml:space="preserve">Based on your own assessment, your grade is in the range:</t>
@@ -809,9 +809,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1294560</xdr:colOff>
+      <xdr:colOff>1294200</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>341640</xdr:rowOff>
+      <xdr:rowOff>341280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -821,7 +821,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6667200" y="1524600"/>
-          <a:ext cx="4241880" cy="694080"/>
+          <a:ext cx="4241520" cy="693720"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
           <a:avLst>
@@ -890,9 +890,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1312920</xdr:colOff>
+      <xdr:colOff>1312560</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -902,7 +902,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7657920" y="552960"/>
-          <a:ext cx="3269520" cy="791280"/>
+          <a:ext cx="3269160" cy="790920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -962,15 +962,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>9360</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:colOff>-720</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>64800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>5037840</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:colOff>5027400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1873440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -979,8 +979,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11959560" y="3743280"/>
-          <a:ext cx="7876800" cy="1907280"/>
+          <a:off x="11949480" y="3432960"/>
+          <a:ext cx="7877160" cy="2179440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1019,7 +1019,7 @@
               <a:latin typeface="Calibri"/>
               <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
-            <a:t>Added the following static routes:</a:t>
+            <a:t>Added 3 static routes:</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1129,7 +1129,7 @@
               <a:latin typeface="Calibri"/>
               <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
-            <a:t>Also added parameterised routes (movies and actors are internally linked):</a:t>
+            <a:t>Added 6 parameterised routes (movies and actors are internally linked):</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1189,7 +1189,7 @@
               <a:latin typeface="Calibri"/>
               <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
-            <a:t>/movie/:id/credits (the list of cast for a movie - movieDetailsPage.jsx)</a:t>
+            <a:t>/movie/:id/credits (the list of cast for a movie – movieDetailsPage.jsx) (Shows age and total movies)</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1219,7 +1219,7 @@
               <a:latin typeface="Calibri"/>
               <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
-            <a:t>/movie/:id/recommendations (list of recommended movies – movieDetailsPage.jsx</a:t>
+            <a:t>/movie/:id/recommendations (list of recommended movies – movieDetailsPage.jsx)</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1279,7 +1279,37 @@
               <a:latin typeface="Calibri"/>
               <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
-            <a:t>/person:id/moviecredits (display movies actor has starred in – personDetailsPage.jsx)</a:t>
+            <a:t>/person:id/moviecredits (display movies actor has starred in / known for – personDetailsPage.jsx)</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:rPr>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:rPr>
+            <a:t>/search/movie?query=:query&amp;page=:page (search functionality to find any movie – searchPage.jsx)</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1298,9 +1328,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>5037840</xdr:colOff>
+      <xdr:colOff>5037480</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1310,7 +1340,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11959560" y="6196680"/>
-          <a:ext cx="7876800" cy="1907280"/>
+          <a:ext cx="7877160" cy="1906920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1409,7 +1439,37 @@
               <a:latin typeface="Calibri"/>
               <a:ea typeface="DejaVu Sans"/>
             </a:rPr>
-            <a:t>Can search for movies or actors. Can filter movies alphabetically, release date rating or popularity. Can filter people alphabetically, age or total movie count</a:t>
+            <a:t>Can search for any movie. </a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:rPr>
+            <a:t>Can filter movies alphabetically, release date rating or popularity on all pages.</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1428,9 +1488,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>5033160</xdr:colOff>
+      <xdr:colOff>5032800</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1902600</xdr:rowOff>
+      <xdr:rowOff>1902240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1440,7 +1500,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11954880" y="8636040"/>
-          <a:ext cx="7876800" cy="1902600"/>
+          <a:ext cx="7877160" cy="1902240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1491,16 +1551,36 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-GB" sz="1100" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="DejaVu Sans"/>
-            </a:rPr>
-            <a:t>Replaced the image on filter card.</a:t>
-          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:rPr>
+            <a:t>Replaced the image on filter card and changed format/location of filter card</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
@@ -1531,15 +1611,55 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-GB" sz="1100" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="DejaVu Sans"/>
-            </a:rPr>
-            <a:t>Used MUI pagination component to display numbers. </a:t>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:rPr>
+            <a:t>Used MUI pagination component to display total pages and current page</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:rPr>
+            <a:t>Changed how favourites worked so you can add and remove without entering favourites tab. Different icon also</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1558,9 +1678,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>5033160</xdr:colOff>
+      <xdr:colOff>5032800</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>1902600</xdr:rowOff>
+      <xdr:rowOff>1902240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1570,7 +1690,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11954880" y="11084760"/>
-          <a:ext cx="7876800" cy="1902240"/>
+          <a:ext cx="7877160" cy="1901880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1755,8 +1875,8 @@
   </sheetPr>
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1766,7 +1886,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="18.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="2" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="12.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="40.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="40.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="80.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="1" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="34.73"/>
@@ -1841,7 +1961,7 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="n">
-        <v>20012345</v>
+        <v>20105917</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>

</xml_diff>